<commit_message>
v0.2 programming from FTDI cable
</commit_message>
<xml_diff>
--- a/docs/satshakit_BOM.xlsx
+++ b/docs/satshakit_BOM.xlsx
@@ -172,7 +172,7 @@
     <t>pin header</t>
   </si>
   <si>
-    <t>POWER</t>
+    <t>POWER/PAD_B</t>
   </si>
   <si>
     <t>M20-9990246</t>
@@ -283,7 +283,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="13.29"/>
+    <col customWidth="1" min="1" max="1" width="14.43"/>
     <col customWidth="1" min="2" max="2" width="12.0"/>
     <col customWidth="1" min="3" max="3" width="38.86"/>
     <col customWidth="1" min="4" max="4" width="19.14"/>
@@ -655,7 +655,7 @@
         <v>0.0525</v>
       </c>
       <c r="H12" s="2">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="I12" s="4">
         <v>0.52</v>

</xml_diff>